<commit_message>
Save gene lists and deleted untitled folder
</commit_message>
<xml_diff>
--- a/RandomForest/CV/Metrics.xlsx
+++ b/RandomForest/CV/Metrics.xlsx
@@ -5,20 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IdentificationOfTSG-OG\TSG_OG_classifier\RandomForest\CV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IdentifyTSGOG\RandomForest\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="New" sheetId="2" r:id="rId2"/>
     <sheet name="OLd" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Consolidated" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -192,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -201,6 +200,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,13 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:Q16"/>
+  <dimension ref="A4:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:Q16"/>
+      <selection activeCell="E17" sqref="E17:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
@@ -830,19 +834,19 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <f>AVERAGE(D5:D14)</f>
         <v>0.86136000000000001</v>
       </c>
-      <c r="E15">
-        <f t="shared" ref="E15:G16" si="0">AVERAGE(E5,E7,E9,E11,E13)</f>
+      <c r="E15" s="1">
+        <f>AVERAGE(E5,E7,E9,E11,E13)</f>
         <v>0.77384000000000008</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
+      <c r="F15" s="1">
+        <f t="shared" ref="E15:G16" si="0">AVERAGE(F5,F7,F9,F11,F13)</f>
         <v>0.92915999999999987</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>0.66505999999999987</v>
       </c>
@@ -852,19 +856,19 @@
       <c r="M15" t="s">
         <v>5</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="1">
         <f>AVERAGE(N5:N14)</f>
         <v>0.76083999999999996</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <f t="shared" ref="O15:Q16" si="1">AVERAGE(O5,O7,O9,O11,O13)</f>
         <v>0.58507999999999993</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="1">
         <f t="shared" si="1"/>
         <v>0.79220000000000002</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="1">
         <f t="shared" si="1"/>
         <v>0.49581999999999998</v>
       </c>
@@ -873,40 +877,94 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89993999999999996</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83792000000000011</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.97241999999999995</v>
+      </c>
+      <c r="M16" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="1">
+        <f>_xlfn.STDEV.S(N5:N14)</f>
+        <v>3.1948208087465568E-2</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82987999999999995</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76822000000000001</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.91163999999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D17" s="1">
         <f>_xlfn.STDEV.S(D5:D14)</f>
         <v>3.9685992491054069E-2</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0.89993999999999996</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0.83792000000000011</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>0.97241999999999995</v>
-      </c>
-      <c r="M16" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16">
-        <f>_xlfn.STDEV.S(N5:N14)</f>
-        <v>3.1948208087465568E-2</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="1"/>
-        <v>0.82987999999999995</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="1"/>
-        <v>0.76822000000000001</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>0.91163999999999989</v>
+      <c r="E17" s="1">
+        <f>_xlfn.STDEV.S(E5,E7,E9,E11,E13)</f>
+        <v>7.273426290270632E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17:G18" si="2">_xlfn.STDEV.S(F5,F7,F9,F11,F13)</f>
+        <v>4.1832857899024779E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>8.8916157136934695E-2</v>
+      </c>
+      <c r="O17" s="1">
+        <f>_xlfn.STDEV.S(O5,O7,O9,O11,O13)</f>
+        <v>0.10395206587653791</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" ref="P17:Q17" si="3">_xlfn.STDEV.S(P5,P7,P9,P11,P13)</f>
+        <v>0.11919389665582648</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="3"/>
+        <v>0.18597154889928744</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <f>_xlfn.STDEV.S(E6,E8,E10,E12,E14)</f>
+        <v>2.7020140636199508E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>3.7799695765971447E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4562863729363152E-2</v>
+      </c>
+      <c r="O18" s="1">
+        <f>_xlfn.STDEV.S(O6,O8,O10,O12,O14)</f>
+        <v>1.6040791751032731E-2</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" ref="P18:Q18" si="4">_xlfn.STDEV.S(P6,P8,P10,P12,P14)</f>
+        <v>6.6262334700793624E-2</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="4"/>
+        <v>6.7441774887676262E-2</v>
       </c>
     </row>
   </sheetData>
@@ -917,10 +975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:Q19"/>
+  <dimension ref="A7:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18:Q19"/>
+      <selection activeCell="D20" sqref="D20:Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1266,71 +1324,151 @@
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D18">
+      <c r="D18" s="1">
         <f>AVERAGE(D8:D17)</f>
         <v>0.83097999999999994</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <f t="shared" ref="E18:G19" si="0">AVERAGE(E8,E10,E12,E14,E16)</f>
         <v>0.71787999999999996</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>0.90454000000000012</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <f t="shared" si="0"/>
         <v>0.59748000000000001</v>
       </c>
-      <c r="N18">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1">
         <f>AVERAGE(N8:N17)</f>
         <v>0.67212000000000005</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="1">
         <f t="shared" ref="O18:Q19" si="1">AVERAGE(O8,O10,O12,O14,O16)</f>
         <v>0.44420000000000004</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="1">
         <f t="shared" si="1"/>
         <v>0.59919999999999995</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="1">
         <f t="shared" si="1"/>
         <v>0.37918000000000002</v>
       </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D19">
+      <c r="D19" s="1">
         <f>_xlfn.STDEV.S(D8:D17)</f>
         <v>1.607877482894763E-2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>0.87919999999999998</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <f t="shared" si="0"/>
         <v>0.80906</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <f t="shared" si="0"/>
         <v>0.96319999999999995</v>
       </c>
-      <c r="N19">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1">
         <f>_xlfn.STDEV.S(N8:N17)</f>
         <v>6.1897512066318133E-2</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="1">
         <f t="shared" si="1"/>
         <v>0.76402000000000003</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="1">
         <f t="shared" si="1"/>
         <v>0.70777999999999996</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="1">
         <f t="shared" si="1"/>
         <v>0.83861999999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
+        <f>_xlfn.STDEV.S(E8,E10,E12,E14,E16)</f>
+        <v>3.4858026335408056E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ref="F20:G21" si="2">_xlfn.STDEV.S(F8,F10,F12,F14,F16)</f>
+        <v>4.4024288750643077E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>4.9603296261438112E-2</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1">
+        <f>_xlfn.STDEV.S(O8,O10,O12,O14,O16)</f>
+        <v>0.12872480335972547</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" ref="P20:Q21" si="3">_xlfn.STDEV.S(P8,P10,P12,P14,P16)</f>
+        <v>0.1863390324113551</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="3"/>
+        <v>0.16265889769699043</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <f>_xlfn.STDEV.S(E9,E11,E13,E15,E17)</f>
+        <v>1.0670520137275423E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7318718197372438E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9693399909614391E-2</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1">
+        <f>_xlfn.STDEV.S(O9,O11,O13,O15,O17)</f>
+        <v>4.9057384765191052E-2</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="3"/>
+        <v>4.9284855686102989E-2</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.10566398156420251</v>
       </c>
     </row>
   </sheetData>
@@ -1343,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="N9:Q9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1780,35 +1918,41 @@
       <c r="C20" t="s">
         <v>38</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <f>AVERAGE(D10:D19)</f>
         <v>0.84045999999999998</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f t="shared" ref="E20:G21" si="0">AVERAGE(E10,E12,E14,E16,E18)</f>
         <v>0.75038000000000005</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <f t="shared" si="0"/>
         <v>0.86069999999999991</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f t="shared" si="0"/>
         <v>0.66916000000000009</v>
       </c>
-      <c r="N20">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1">
         <f>AVERAGE(N10:N19)</f>
         <v>0.7466799999999999</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="1">
         <f t="shared" ref="O20:Q21" si="1">AVERAGE(O10,O12,O14,O16,O18)</f>
         <v>0.59216000000000002</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="1">
         <f t="shared" si="1"/>
         <v>0.71016000000000001</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="1">
         <f t="shared" si="1"/>
         <v>0.51916000000000007</v>
       </c>
@@ -1817,37 +1961,111 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <f>_xlfn.STDEV.S(D10:D19)</f>
         <v>4.5517502128302252E-2</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>0.88257999999999992</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <f t="shared" si="0"/>
         <v>0.83452000000000004</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <f t="shared" si="0"/>
         <v>0.93756000000000006</v>
       </c>
-      <c r="N21">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1">
         <f>_xlfn.STDEV.S(N10:N19)</f>
         <v>4.3920177595269359E-2</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="1">
         <f t="shared" si="1"/>
         <v>0.81501999999999997</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="1">
         <f t="shared" si="1"/>
         <v>0.76506000000000007</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="1">
         <f t="shared" si="1"/>
         <v>0.87540000000000018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
+        <f>_xlfn.STDEV.S(E10,E12,E14,E16,E18)</f>
+        <v>7.4470410231178383E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" ref="F22:G23" si="2">_xlfn.STDEV.S(F10,F12,F14,F16,F18)</f>
+        <v>7.5124962562386668E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>9.0960419963848682E-2</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1">
+        <f>_xlfn.STDEV.S(O10,O12,O14,O16,O18)</f>
+        <v>9.4784297222693353E-2</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" ref="P22:Q23" si="3">_xlfn.STDEV.S(P10,P12,P14,P16,P18)</f>
+        <v>0.107129211702505</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="3"/>
+        <v>0.12119962046145168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
+        <f>_xlfn.STDEV.S(E11,E13,E15,E17,E19)</f>
+        <v>3.3281105750861094E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="2"/>
+        <v>4.0465750950649602E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="2"/>
+        <v>3.8526393550396047E-2</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1">
+        <f>_xlfn.STDEV.S(O11,O13,O15,O17,O19)</f>
+        <v>3.1401066860856808E-2</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="3"/>
+        <v>4.1003451074269351E-2</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="3"/>
+        <v>6.0470281957338348E-2</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
@@ -3027,21 +3245,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P9"/>
+  <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
@@ -3076,7 +3310,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C4" t="s">
@@ -3097,7 +3331,7 @@
       <c r="H4" s="1">
         <v>0.66505999999999987</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K4" t="s">
@@ -3120,6 +3354,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -3134,6 +3369,7 @@
       <c r="H5" s="1">
         <v>0.97241999999999995</v>
       </c>
+      <c r="J5" s="2"/>
       <c r="K5" t="s">
         <v>6</v>
       </c>
@@ -3150,7 +3386,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
@@ -3171,7 +3407,7 @@
       <c r="H6" s="1">
         <v>0.59748000000000001</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="K6" t="s">
@@ -3194,6 +3430,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -3208,6 +3445,7 @@
       <c r="H7" s="1">
         <v>0.96319999999999995</v>
       </c>
+      <c r="J7" s="2"/>
       <c r="K7" t="s">
         <v>6</v>
       </c>
@@ -3224,7 +3462,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C8" t="s">
@@ -3245,7 +3483,7 @@
       <c r="H8" s="1">
         <v>0.66916000000000009</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="K8" t="s">
@@ -3268,6 +3506,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -3282,6 +3521,7 @@
       <c r="H9" s="1">
         <v>0.93756000000000006</v>
       </c>
+      <c r="J9" s="2"/>
       <c r="K9" t="s">
         <v>6</v>
       </c>
@@ -3297,12 +3537,138 @@
         <v>0.87540000000000018</v>
       </c>
     </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="J13" s="4"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="J14" s="4"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="J15" s="4"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="J16" s="4"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="J17" s="4"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="J18" s="4"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="D4:D5"/>
+  <mergeCells count="20">
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="L4:L5"/>
@@ -3311,6 +3677,18 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>